<commit_message>
Tentando escrever na tabela
</commit_message>
<xml_diff>
--- a/php/exemplo.xlsx
+++ b/php/exemplo.xlsx
@@ -111,6 +111,33 @@
         </is>
       </c>
     </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>137463</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>COMPREHENDING THE TRANSPORT PROPERTIES OF PROTIC IONIC LIQUIDS USING NMR</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>Poster Presentation</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>Andrea Mele;</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>Department of Chemistry, Materials and Chemical Engineering “Giulio Natta” / Politecnico di Milano</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>